<commit_message>
add logging and tokens are configurable
</commit_message>
<xml_diff>
--- a/output/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings.xlsx
+++ b/output/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings/3.5._Manufacture_of_energy_efficiency_equipment_for_buildings.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="No_Valid_Sections" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CCM_3.5" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,912 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>No valid sections were generated for this activity.</t>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>3.5. Manufacture of energy efficiency equipment for buildings</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DNSH Goal</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Substantial Contribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Product &amp; Project</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Formula IDs</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>((ePBN111002_1|ePBN111003_1|ePBN115700_1|ePBN115701_1|ePBN115699_1|ePBN115691_1|ePBN115692_1|ePBN115693_1|ePBN115694_1|ePBN115695_1|ePBN115696_1|ePBN115697_1|ePBN115698_1|ePBN115690_1|ePBN115688_1|ePBN115689_1|ePBN115687_1))&amp;(ePBN993847_1&lt;&gt;1)&amp;ePBN110911_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Formula Display</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>((m) energy-efficient building automation and control systems for residential and non-residential buildings|n) zoned thermostats and devices for the smart monitoring of the main electricity loads or heat loads for buildings, and sensoring equipment|p) district heating exchangers and substations compliant with the district heating/cooling distribution activity set out in Section 4.15 of this Annex;|q) products for smart monitoring and regulating of heating system, and sensoring equipment.|o) products for heat metering and thermostatic controls for individual homes connected to district heating systems, for individual flats connected to central heating systems serving a whole building, and for central heating systems;|e) insulating products with a lambda value lower or equal to 0,06 W/mK|f) household appliances falling into the highest two populated classes of energy efficiency in accordance with Regulation (EU) 2017/1369 of the European Parliament and of the Council (95) and delegated acts adopted under that Regulation;|g) light sources rated in the highest two populated classes of energy efficiency in accordance with Regulation (EU) 2017/1369 and delegated acts adopted under that Regulation;|h) space heating and domestic hot water systems rated in the highest two populated classes of energy efficiency in accordance with Regulation (EU) 2017/1369 and delegated acts adopted under that Regulation;|i) cooling and ventilation systems rated in the highest two populated classes of energy efficiency in accordance with Regulation (EU) 2017/1369 and delegated acts adopted under that Regulation;|j) presence and daylight controls for lighting systems;|k) heat pumps compliant with the technical screening criteria set out in Section 4.16 of this Annex;|l) façade and roofing elements with a solar shading or solar control function, including those that support the growing of vegetation;|d) roofing systems with U-value lower or equal to 0,3 W/m2K;|b) doors with U-value lower or equal to 1,2 W/m2K;|c) external wall systems with U-value lower or equal to 0,5 W/m2K;|a) windows with U-value lower or equal to 1,0 W/m2K;))&amp;(CCM 3.5: No substantial contribution. The assessment is considered complete despite missing answers.&lt;&gt;1)&amp;3.5. Manufacture of energy efficiency equipment for buildings</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Variable ID</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 3</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 4</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 5</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 6</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 7</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 8</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 9</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 10</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 11</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 12</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 13</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 14</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 15</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 16</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Alignment Rule 17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ePBN110911_1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ePBN110911_1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ePBN111002_1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ePBN111002_1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ePBN111003_1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ePBN111003_1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ePBN115687_1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ePBN115687_1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ePBN115688_1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ePBN115688_1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ePBN115689_1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ePBN115689_1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ePBN115690_1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ePBN115690_1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ePBN115691_1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ePBN115691_1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ePBN115692_1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ePBN115692_1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ePBN115693_1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ePBN115693_1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ePBN115694_1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ePBN115694_1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ePBN115695_1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ePBN115695_1</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ePBN115696_1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>ePBN115696_1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ePBN115697_1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ePBN115697_1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ePBN115698_1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ePBN115698_1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ePBN115699_1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ePBN115699_1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ePBN115700_1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ePBN115700_1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ePBN115701_1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ePBN115701_1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ePBN993847_1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ePBN993847_1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Not Yes</t>
         </is>
       </c>
     </row>

</xml_diff>